<commit_message>
zweite Welle wieder gelöscht
</commit_message>
<xml_diff>
--- a/data/instruments/instruments.xlsx
+++ b/data/instruments/instruments.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="66">
   <si>
     <t>number</t>
   </si>
@@ -213,12 +213,6 @@
   </si>
   <si>
     <t>subtitle.en</t>
-  </si>
-  <si>
-    <t>Fragebogen des DZHW-Absolventenpanels 2009 - zweite Welle</t>
-  </si>
-  <si>
-    <t>Questionnaire of DZHW Graduate Panel 2009 - second wave</t>
   </si>
 </sst>
 </file>
@@ -632,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,20 +699,6 @@
         <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G3" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>